<commit_message>
Ajout QR au flux 1 82b150d37acbb590ddc08537cc191beec8e9e9a9
</commit_message>
<xml_diff>
--- a/361-Flux-Mise-à-jour-du-flux-1/ig/StructureDefinition-tddui-patient-ins.xlsx
+++ b/361-Flux-Mise-à-jour-du-flux-1/ig/StructureDefinition-tddui-patient-ins.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-24T14:08:52+00:00</t>
+    <t>2025-10-01T08:29:05+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -5769,7 +5769,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" hidden="true">
+    <row r="23">
       <c r="A23" t="s" s="2">
         <v>221</v>
       </c>
@@ -13579,7 +13579,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="88" hidden="true">
+    <row r="88">
       <c r="A88" t="s" s="2">
         <v>487</v>
       </c>
@@ -16831,7 +16831,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="115" hidden="true">
+    <row r="115">
       <c r="A115" t="s" s="2">
         <v>529</v>
       </c>
@@ -20445,7 +20445,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="145" hidden="true">
+    <row r="145">
       <c r="A145" t="s" s="2">
         <v>644</v>
       </c>
@@ -20805,7 +20805,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="148" hidden="true">
+    <row r="148">
       <c r="A148" t="s" s="2">
         <v>650</v>
       </c>
@@ -21887,7 +21887,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="157" hidden="true">
+    <row r="157">
       <c r="A157" t="s" s="2">
         <v>676</v>
       </c>
@@ -22007,7 +22007,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="158" hidden="true">
+    <row r="158">
       <c r="A158" t="s" s="2">
         <v>686</v>
       </c>
@@ -26223,12 +26223,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AP192">
-    <filterColumn colId="6">
+    <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <filterColumn colId="26">
+    <filterColumn colId="27">
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>

</xml_diff>